<commit_message>
Switched on the "L1_DoubleMu18er2p1_SQ" seed
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-13.6TeV_2748b.xlsx
+++ b/official/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-13.6TeV_2748b.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_2_0_off/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F157B8-B84E-B94E-8728-5A24EEF19824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3307C1ED-FD62-4C49-8D1A-280B14B1934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1884,10 +1884,10 @@
   <dimension ref="A1:K1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3602,28 +3602,28 @@
         <v>0</v>
       </c>
       <c r="D50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -20091,32 +20091,32 @@
       <c r="K1010" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:C370 I3:I370 K3:K398 E3:E84 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392">
+  <conditionalFormatting sqref="C3:C370 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392 I3:I370 K3:K398 E3:E84">
     <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C370 I3:I370 K3:K398 E3:E84 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392">
+  <conditionalFormatting sqref="C3:C370 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392 I3:I370 K3:K398 E3:E84">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C370 I3:I370 K3:K398 E3:E84 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392">
+  <conditionalFormatting sqref="C3:C370 E86:E232 E236:E370 E381:E391 I381:I391 C381:C599 C380:J380 I372:I379 E372:E379 C372:C379 C371:J371 I393:I398 E393:E599 D392:J392 I3:I370 K3:K398 E3:E84">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J174 J177:J370 J381:J391 J372:J379 J393:J398">
+  <conditionalFormatting sqref="J177:J370 J381:J391 J372:J379 J393:J398 J3:J174">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J174 J177:J370 J381:J391 J372:J379 J393:J398">
+  <conditionalFormatting sqref="J177:J370 J381:J391 J372:J379 J393:J398 J3:J174">
     <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J174 J177:J370 J381:J391 J372:J379 J393:J398">
+  <conditionalFormatting sqref="J177:J370 J381:J391 J372:J379 J393:J398 J3:J174">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
@@ -20136,62 +20136,62 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H370 H381:H391 H372:H379 H393:H398">
+  <conditionalFormatting sqref="H381:H391 H372:H379 H393:H398 H3:H370">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H370 H381:H391 H372:H379 H393:H398">
+  <conditionalFormatting sqref="H381:H391 H372:H379 H393:H398 H3:H370">
     <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H370 H381:H391 H372:H379 H393:H398">
+  <conditionalFormatting sqref="H381:H391 H372:H379 H393:H398 H3:H370">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G370 G381:G391 G372:G379 G393:G398">
+  <conditionalFormatting sqref="G381:G391 G372:G379 G393:G398 G3:G370">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G370 G381:G391 G372:G379 G393:G398">
+  <conditionalFormatting sqref="G381:G391 G372:G379 G393:G398 G3:G370">
     <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G370 G381:G391 G372:G379 G393:G398">
+  <conditionalFormatting sqref="G381:G391 G372:G379 G393:G398 G3:G370">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F370 F381:F391 F372:F379 F393:F398">
+  <conditionalFormatting sqref="F381:F391 F372:F379 F393:F398 F3:F370">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F370 F381:F391 F372:F379 F393:F398">
+  <conditionalFormatting sqref="F381:F391 F372:F379 F393:F398 F3:F370">
     <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F370 F381:F391 F372:F379 F393:F398">
+  <conditionalFormatting sqref="F381:F391 F372:F379 F393:F398 F3:F370">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D232 D235:D370 D381:D391 D372:D379 D393:D599">
+  <conditionalFormatting sqref="D235:D370 D381:D391 D372:D379 D393:D599 D3:D232">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D232 D235:D370 D381:D391 D372:D379 D393:D599">
+  <conditionalFormatting sqref="D235:D370 D381:D391 D372:D379 D393:D599 D3:D232">
     <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D232 D235:D370 D381:D391 D372:D379 D393:D599">
+  <conditionalFormatting sqref="D235:D370 D381:D391 D372:D379 D393:D599 D3:D232">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>